<commit_message>
Adjust the manually extracted rule
</commit_message>
<xml_diff>
--- a/artifacts/manually-extracted-rules.xlsx
+++ b/artifacts/manually-extracted-rules.xlsx
@@ -66,7 +66,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">in Application</t>
+      <t xml:space="preserve">in Application class with value “MP-JWT”</t>
     </r>
     <r>
       <rPr>
@@ -87,7 +87,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">use </t>
+      <t xml:space="preserve">then all methods with annotations @GET (and other HTTP anns) must have </t>
     </r>
     <r>
       <rPr>
@@ -98,17 +98,17 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">@RolesAllowed() </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">on target method (GET)</t>
+      <t xml:space="preserve">@RolesAllowed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">as well.</t>
     </r>
   </si>
   <si>
@@ -660,11 +660,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -673,16 +669,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -779,14 +767,14 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1020" min="6" style="0" width="14.43"/>
@@ -794,292 +782,292 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+    <row r="2" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="8" t="s">
+      <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="102.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="4" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>